<commit_message>
Push covid timeline code and figure.
</commit_message>
<xml_diff>
--- a/covid-test-results.xlsx
+++ b/covid-test-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelflynn/Dropbox/KANSAS/COVID Stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478865F4-D33D-E149-B9C0-52CB3D7BD238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAE862A-385B-C440-B988-EAC6CD320394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{7687D1C1-6504-1049-BE14-339D59436FD7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,34 +688,144 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2">
+        <v>44738</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2">
+        <v>44740</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2">
+        <v>44740</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2">
+        <v>44740</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2">
+        <v>44736</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2">
+        <v>44737</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2">
+        <v>44742</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2">
+        <v>44744</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2">
+        <v>44742</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2">
+        <v>44737</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>